<commit_message>
remove unuse prop. change org account demo file.
</commit_message>
<xml_diff>
--- a/VMS/wwwroot/files/admin/IMPORT_ORG_DEMO.xlsx
+++ b/VMS/wwwroot/files/admin/IMPORT_ORG_DEMO.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tranv\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D09A1A35-213F-40FE-A40A-8AFA3F79883F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0318B25F-7683-4F9E-8DDC-011927972FFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Trang tính1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>STT</t>
   </si>
@@ -34,15 +34,6 @@
     <t>CẤP</t>
   </si>
   <si>
-    <t>CLB BẠN GÁI</t>
-  </si>
-  <si>
-    <t>CLB</t>
-  </si>
-  <si>
-    <t>BAN CHUYÊN MÔN</t>
-  </si>
-  <si>
     <t>org.001@gmail.com</t>
   </si>
   <si>
@@ -59,13 +50,34 @@
   </si>
   <si>
     <t>WHEREareU</t>
+  </si>
+  <si>
+    <t>Ban Chuyên môn</t>
+  </si>
+  <si>
+    <t>Khoa/Viện/KTX</t>
+  </si>
+  <si>
+    <t>org.003@gmail.com</t>
+  </si>
+  <si>
+    <t>KTX 135</t>
+  </si>
+  <si>
+    <t>BAN PHONG TRÀO TÌNH NGUYỆN</t>
+  </si>
+  <si>
+    <t>CLB/Đội/Nhóm</t>
+  </si>
+  <si>
+    <t>DontKnowWTODO</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -85,6 +97,11 @@
       <sz val="10"/>
       <color theme="10"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -123,7 +140,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -132,6 +149,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -353,17 +373,17 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="6.85546875" customWidth="1"/>
     <col min="2" max="2" width="29.42578125" customWidth="1"/>
-    <col min="3" max="3" width="18" customWidth="1"/>
+    <col min="3" max="3" width="39.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="25.5703125" customWidth="1"/>
     <col min="5" max="5" width="23" bestFit="1" customWidth="1"/>
   </cols>
@@ -382,7 +402,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -390,16 +410,16 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="2" t="s">
         <v>4</v>
       </c>
+      <c r="C2" s="4" t="s">
+        <v>14</v>
+      </c>
       <c r="D2" s="2" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -407,23 +427,42 @@
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="2" t="s">
+    </row>
+    <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="2">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>12</v>
+      <c r="D4" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{0055D12A-539A-4716-BAA1-15754C652AC3}"/>
     <hyperlink ref="B3" r:id="rId2" xr:uid="{744A39B6-F655-41DE-8D6A-07D888D8E3AC}"/>
+    <hyperlink ref="B4" r:id="rId3" xr:uid="{CD49C438-87D2-489B-AF64-8CCDB786D340}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>